<commit_message>
gearbox and motor data updated
</commit_message>
<xml_diff>
--- a/Motors.xlsx
+++ b/Motors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\1 - Personal\Programming\Projects\Gearbox_Selection\Gearbox_Selection_1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\1 - Personal\Programming\Python\Projects\Gearbox_Selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B132408-1EF1-4EA7-B5EB-5F320123D9F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A01CCD-4C00-44FE-BD49-1E8B940A915A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2 Pole" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="49">
   <si>
     <t>Motor Information</t>
   </si>
@@ -127,9 +127,6 @@
     <t>BN</t>
   </si>
   <si>
-    <t>BE</t>
-  </si>
-  <si>
     <t>MAX-E3</t>
   </si>
   <si>
@@ -182,13 +179,22 @@
   </si>
   <si>
     <t>250M</t>
+  </si>
+  <si>
+    <t>132SB</t>
+  </si>
+  <si>
+    <t>132MA</t>
+  </si>
+  <si>
+    <t>BX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +228,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -392,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -428,15 +440,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -486,6 +489,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,9 +787,7 @@
   </sheetPr>
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -788,15 +801,15 @@
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -823,16 +836,16 @@
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="11" t="s">
@@ -854,28 +867,28 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="16">
         <v>0.18</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="22">
         <v>2730</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="25">
-        <v>11</v>
-      </c>
-      <c r="E3" s="25">
+      <c r="D3" s="22">
+        <v>11</v>
+      </c>
+      <c r="E3" s="22">
         <v>3.5</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="20"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -883,28 +896,28 @@
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="18">
         <v>0.25</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="14">
         <v>2740</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="17">
-        <v>11</v>
-      </c>
-      <c r="E4" s="17">
+      <c r="D4" s="14">
+        <v>11</v>
+      </c>
+      <c r="E4" s="14">
         <v>3.9</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -912,28 +925,28 @@
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="18">
         <v>0.37</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="14">
         <v>2820</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="14">
         <v>14</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="14">
         <v>5.4</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="19" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="4"/>
@@ -943,28 +956,28 @@
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26">
+      <c r="A6" s="23">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="24">
         <v>2820</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="24">
         <v>14</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="24">
         <v>6.2</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="24"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -972,28 +985,28 @@
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="13">
         <v>0.75</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="14">
         <v>2880</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="14">
         <v>80</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="14">
         <v>19</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <v>9.5</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="22"/>
+      <c r="G7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="19"/>
       <c r="I7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -1001,28 +1014,28 @@
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="A8" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="14">
         <v>2880</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="14">
         <v>80</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="14">
         <v>19</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="22"/>
+      <c r="G8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="19"/>
       <c r="I8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -1030,28 +1043,28 @@
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+      <c r="A9" s="13">
         <v>1.5</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="14">
         <v>2870</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="17">
+      <c r="C9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="14">
         <v>24</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="22"/>
+      <c r="G9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="19"/>
       <c r="I9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -1059,28 +1072,28 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="13">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="14">
         <v>2870</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="14">
         <v>24</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>17</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="22"/>
+      <c r="G10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="19"/>
       <c r="I10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -1088,28 +1101,28 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="13">
         <v>3</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="14">
         <v>2900</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="17">
-        <v>28</v>
-      </c>
-      <c r="E11" s="17">
+      <c r="D11" s="14">
+        <v>28</v>
+      </c>
+      <c r="E11" s="14">
         <v>24.5</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="22"/>
+      <c r="G11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="19"/>
       <c r="I11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -1117,28 +1130,28 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="A12" s="13">
         <v>4</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="14">
         <v>2920</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="17">
-        <v>28</v>
-      </c>
-      <c r="E12" s="17">
+      <c r="D12" s="14">
+        <v>28</v>
+      </c>
+      <c r="E12" s="14">
         <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="22"/>
+      <c r="G12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="19"/>
       <c r="I12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -1146,28 +1159,28 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="16">
         <v>5.5</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="22">
         <v>2930</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="25">
+      <c r="C13" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="22">
         <v>38</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="22">
         <v>75</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="20"/>
+      <c r="G13" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="17"/>
       <c r="I13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -1175,14 +1188,14 @@
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="18">
         <v>7.5</v>
       </c>
       <c r="B14" s="2">
         <v>2920</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2">
         <v>27</v>
@@ -1194,12 +1207,12 @@
         <v>11</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="18">
         <v>11</v>
       </c>
       <c r="B15" s="2">
@@ -1218,12 +1231,12 @@
         <v>11</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="18">
         <v>15</v>
       </c>
       <c r="B16" s="2">
@@ -1242,19 +1255,19 @@
         <v>11</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="18">
         <v>18.5</v>
       </c>
       <c r="B17" s="2">
         <v>2940</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2">
         <v>42</v>
@@ -1266,19 +1279,19 @@
         <v>11</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="18">
         <v>22</v>
       </c>
       <c r="B18" s="2">
         <v>2950</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2">
         <v>48</v>
@@ -1290,19 +1303,19 @@
         <v>11</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="18">
         <v>30</v>
       </c>
       <c r="B19" s="2">
         <v>2945</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="2">
         <v>55</v>
@@ -1314,19 +1327,19 @@
         <v>11</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="18">
         <v>37</v>
       </c>
       <c r="B20" s="2">
         <v>2960</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2">
         <v>55</v>
@@ -1338,19 +1351,19 @@
         <v>11</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23">
+      <c r="A21" s="20">
         <v>45</v>
       </c>
       <c r="B21" s="9">
         <v>2960</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="9">
         <v>55</v>
@@ -1362,9 +1375,9 @@
         <v>11</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="24"/>
+        <v>28</v>
+      </c>
+      <c r="H21" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1382,9 +1395,7 @@
   </sheetPr>
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1398,15 +1409,15 @@
       <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -1433,16 +1444,16 @@
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="11" t="s">
@@ -1464,28 +1475,28 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="16">
         <v>0.06</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="22">
         <v>1340</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="25">
+      <c r="C3" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="22">
         <v>9</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="22">
         <v>3.1</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="20"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1493,28 +1504,28 @@
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="18">
         <v>0.09</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="14">
         <v>1350</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="17">
+      <c r="C4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="14">
         <v>9</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="14">
         <v>3.1</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -1522,28 +1533,28 @@
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="A5" s="13">
         <v>0.12</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="14">
         <v>1350</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="17">
-        <v>11</v>
-      </c>
-      <c r="E5" s="17">
+      <c r="D5" s="14">
+        <v>11</v>
+      </c>
+      <c r="E5" s="14">
         <v>3.5</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -1551,28 +1562,28 @@
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="13">
         <v>0.18</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>1320</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="17">
-        <v>11</v>
-      </c>
-      <c r="E6" s="17">
+      <c r="D6" s="14">
+        <v>11</v>
+      </c>
+      <c r="E6" s="14">
         <v>3.9</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -1580,28 +1591,28 @@
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="13">
         <v>0.25</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="14">
         <v>1380</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="14">
         <v>14</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <v>5.0999999999999996</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="19" t="s">
         <v>19</v>
       </c>
       <c r="I7" s="4"/>
@@ -1611,28 +1622,28 @@
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="A8" s="13">
         <v>0.37</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="14">
         <v>1370</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="14">
         <v>14</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>5.9</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="19"/>
       <c r="I8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -1640,28 +1651,28 @@
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23">
+      <c r="A9" s="20">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="24">
         <v>1400</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="24">
         <v>19</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="24">
         <v>9.9</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="21" t="s">
         <v>18</v>
       </c>
       <c r="I9" s="4"/>
@@ -1671,28 +1682,28 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
+      <c r="A10" s="25">
         <v>0.75</v>
       </c>
-      <c r="B10" s="25">
-        <v>1430</v>
-      </c>
-      <c r="C10" s="25" t="s">
+      <c r="B10" s="22">
+        <v>1425</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <v>19</v>
       </c>
-      <c r="E10" s="25">
-        <v>12.2</v>
+      <c r="E10" s="22">
+        <v>16</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="20"/>
+      <c r="G10" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="17"/>
       <c r="I10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -1700,28 +1711,28 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B11" s="17">
-        <v>1430</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="17">
+      <c r="B11" s="14">
+        <v>1425</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="14">
         <v>24</v>
       </c>
-      <c r="E11" s="17">
-        <v>13.6</v>
+      <c r="E11" s="14">
+        <v>16</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="22"/>
+      <c r="G11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="19"/>
       <c r="I11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -1729,28 +1740,28 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="13">
         <v>1.5</v>
       </c>
-      <c r="B12" s="17">
-        <v>1430</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="17">
+      <c r="B12" s="14">
+        <v>1420</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="14">
         <v>24</v>
       </c>
-      <c r="E12" s="17">
-        <v>15.1</v>
+      <c r="E12" s="14">
+        <v>17</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="22"/>
+      <c r="G12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="19"/>
       <c r="I12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -1758,28 +1769,28 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="A13" s="18">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B13" s="17">
-        <v>1430</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="17">
-        <v>28</v>
-      </c>
-      <c r="E13" s="17">
-        <v>22</v>
+      <c r="B13" s="14">
+        <v>1445</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="14">
+        <v>28</v>
+      </c>
+      <c r="E13" s="14">
+        <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="22"/>
+      <c r="G13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="19"/>
       <c r="I13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -1787,103 +1798,103 @@
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="18">
         <v>3</v>
       </c>
       <c r="B14" s="2">
-        <v>1420</v>
+        <v>1445</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2">
         <v>28</v>
       </c>
       <c r="E14" s="2">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="22"/>
-    </row>
-    <row r="15" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23">
+      <c r="G14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
         <v>4</v>
       </c>
-      <c r="B15" s="9">
-        <v>1440</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="2">
+        <v>1445</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="9">
-        <v>28</v>
-      </c>
-      <c r="E15" s="9">
-        <v>32</v>
-      </c>
-      <c r="F15" s="9" t="s">
+      <c r="D15" s="2">
+        <v>28</v>
+      </c>
+      <c r="E15" s="2">
+        <v>38</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="24"/>
+      <c r="G15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="18">
         <v>5.5</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="2">
+        <v>1470</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="2">
+        <v>38</v>
+      </c>
+      <c r="E16" s="2">
+        <v>57</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20">
+        <v>7.5</v>
+      </c>
+      <c r="B17" s="9">
         <v>1460</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="C17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="9">
         <v>38</v>
       </c>
-      <c r="E16" s="7">
-        <v>75</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
-        <v>7.5</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1465</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="2">
-        <v>38</v>
-      </c>
-      <c r="E17" s="2">
-        <v>82</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="22"/>
+      <c r="E17" s="9">
+        <v>67</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="21"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="18">
         <v>11</v>
       </c>
       <c r="B18" s="2">
@@ -1902,19 +1913,19 @@
         <v>11</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="18">
         <v>15</v>
       </c>
       <c r="B19" s="2">
         <v>1465</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2">
         <v>42</v>
@@ -1926,19 +1937,19 @@
         <v>11</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="18">
         <v>18.5</v>
       </c>
       <c r="B20" s="2">
         <v>1480</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="2">
         <v>48</v>
@@ -1950,19 +1961,19 @@
         <v>11</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="18">
         <v>22</v>
       </c>
       <c r="B21" s="2">
         <v>1480</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2">
         <v>48</v>
@@ -1974,19 +1985,19 @@
         <v>11</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
+      <c r="A22" s="18">
         <v>30</v>
       </c>
       <c r="B22" s="2">
         <v>1475</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="2">
         <v>55</v>
@@ -1998,19 +2009,19 @@
         <v>11</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23" s="18">
         <v>37</v>
       </c>
       <c r="B23" s="2">
         <v>1480</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="2">
         <v>60</v>
@@ -2022,19 +2033,19 @@
         <v>11</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23">
+      <c r="A24" s="20">
         <v>45</v>
       </c>
       <c r="B24" s="9">
         <v>1480</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="9">
         <v>60</v>
@@ -2046,7 +2057,7 @@
         <v>11</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H24" s="10"/>
     </row>
@@ -2055,7 +2066,7 @@
     <mergeCell ref="B1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2066,9 +2077,7 @@
   </sheetPr>
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2082,15 +2091,15 @@
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -2108,28 +2117,28 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="26" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="2"/>
@@ -2148,28 +2157,28 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="16">
         <v>0.09</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="22">
         <v>880</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="25">
-        <v>11</v>
-      </c>
-      <c r="E3" s="25">
+      <c r="D3" s="22">
+        <v>11</v>
+      </c>
+      <c r="E3" s="22">
         <v>4.5999999999999996</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="20"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -2177,28 +2186,28 @@
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="18">
         <v>0.12</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="14">
         <v>870</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="17">
-        <v>11</v>
-      </c>
-      <c r="E4" s="17">
+      <c r="D4" s="14">
+        <v>11</v>
+      </c>
+      <c r="E4" s="14">
         <v>4.9000000000000004</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="3"/>
       <c r="J4" s="2"/>
       <c r="K4" s="4"/>
@@ -2207,7 +2216,7 @@
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="18">
         <v>0.18</v>
       </c>
       <c r="B5" s="2">
@@ -2237,28 +2246,28 @@
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="13">
         <v>0.25</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>900</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="14">
         <v>14</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="14">
         <v>6.7</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="3"/>
       <c r="J6" s="2"/>
       <c r="K6" s="4"/>
@@ -2267,28 +2276,28 @@
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="13">
         <v>0.37</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="14">
         <v>910</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="14">
         <v>19</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <v>9.9</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="19" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="3"/>
@@ -2299,28 +2308,28 @@
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26">
+      <c r="A8" s="23">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="24">
         <v>920</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="24">
         <v>19</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="24">
         <v>11.3</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="24"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="3"/>
       <c r="J8" s="2"/>
       <c r="K8" s="4"/>
@@ -2329,28 +2338,28 @@
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="25">
         <v>0.75</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="22">
         <v>940</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="25">
+      <c r="C9" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="22">
         <v>24</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <v>12.5</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="20"/>
+      <c r="G9" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="17"/>
       <c r="I9" s="3"/>
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
@@ -2359,28 +2368,28 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="14">
         <v>940</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="14">
         <v>24</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>15.5</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="22"/>
+      <c r="G10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="19"/>
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
@@ -2389,28 +2398,28 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="13">
         <v>1.5</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="14">
         <v>950</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="17">
-        <v>28</v>
-      </c>
-      <c r="E11" s="17">
+      <c r="D11" s="14">
+        <v>28</v>
+      </c>
+      <c r="E11" s="14">
         <v>26.5</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="22"/>
+      <c r="G11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="19"/>
       <c r="I11" s="3"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
@@ -2419,28 +2428,28 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="13">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="14">
         <v>950</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="17">
-        <v>28</v>
-      </c>
-      <c r="E12" s="17">
+      <c r="D12" s="14">
+        <v>28</v>
+      </c>
+      <c r="E12" s="14">
         <v>29.5</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="22"/>
+      <c r="G12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="19"/>
       <c r="I12" s="3"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
@@ -2449,28 +2458,28 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+      <c r="A13" s="13">
         <v>3</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="14">
         <v>960</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="17">
+      <c r="C13" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="14">
         <v>38</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="14">
         <v>38.5</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="22"/>
+      <c r="G13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="19"/>
       <c r="I13" s="3"/>
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
@@ -2479,40 +2488,40 @@
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23">
+      <c r="A14" s="20">
         <v>4</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="24">
         <v>960</v>
       </c>
-      <c r="C14" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="27">
+      <c r="C14" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="24">
         <v>38</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="24">
         <v>48</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="24"/>
+      <c r="G14" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="21"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="16">
         <v>5.5</v>
       </c>
       <c r="B15" s="7">
         <v>970</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="7">
         <v>38</v>
@@ -2524,14 +2533,14 @@
         <v>11</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15" s="20"/>
+        <v>28</v>
+      </c>
+      <c r="H15" s="17"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="18">
         <v>7.5</v>
       </c>
       <c r="B16" s="2">
@@ -2550,21 +2559,21 @@
         <v>11</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H16" s="19"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="18">
         <v>11</v>
       </c>
       <c r="B17" s="2">
         <v>965</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2">
         <v>42</v>
@@ -2576,21 +2585,21 @@
         <v>11</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H17" s="19"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="18">
         <v>15</v>
       </c>
       <c r="B18" s="2">
         <v>970</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="2">
         <v>48</v>
@@ -2602,21 +2611,21 @@
         <v>11</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H18" s="19"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="18">
         <v>18.5</v>
       </c>
       <c r="B19" s="2">
         <v>975</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="2">
         <v>55</v>
@@ -2628,21 +2637,21 @@
         <v>11</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H19" s="19"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="18">
         <v>22</v>
       </c>
       <c r="B20" s="2">
         <v>975</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2">
         <v>55</v>
@@ -2654,21 +2663,21 @@
         <v>11</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H20" s="19"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="18">
         <v>30</v>
       </c>
       <c r="B21" s="2">
         <v>985</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2">
         <v>60</v>
@@ -2680,21 +2689,21 @@
         <v>11</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H21" s="19"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
+      <c r="A22" s="18">
         <v>37</v>
       </c>
       <c r="B22" s="2">
         <v>985</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2">
         <v>70</v>
@@ -2706,21 +2715,21 @@
         <v>11</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H22" s="19"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23">
+      <c r="A23" s="20">
         <v>45</v>
       </c>
       <c r="B23" s="9">
         <v>985</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="9">
         <v>70</v>
@@ -2732,7 +2741,7 @@
         <v>11</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="2"/>
@@ -2790,9 +2799,7 @@
   </sheetPr>
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2806,15 +2813,15 @@
       <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -2832,28 +2839,28 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="26" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="2"/>
@@ -2872,14 +2879,28 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="20"/>
+      <c r="A3" s="16">
+        <v>0.18</v>
+      </c>
+      <c r="B3" s="22">
+        <v>705</v>
+      </c>
+      <c r="C3" s="22">
+        <v>80</v>
+      </c>
+      <c r="D3" s="22">
+        <v>19</v>
+      </c>
+      <c r="E3" s="22">
+        <v>16</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="17"/>
       <c r="I3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -2887,14 +2908,28 @@
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="22"/>
+      <c r="A4" s="18">
+        <v>0.37</v>
+      </c>
+      <c r="B4" s="14">
+        <v>710</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="14">
+        <v>24</v>
+      </c>
+      <c r="E4" s="14">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="19"/>
       <c r="I4" s="3"/>
       <c r="J4" s="2"/>
       <c r="K4" s="4"/>
@@ -2903,13 +2938,27 @@
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="18">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B5" s="2">
+        <v>690</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="H5" s="8"/>
       <c r="I5" s="3"/>
       <c r="J5" s="2"/>
@@ -2919,14 +2968,28 @@
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="22"/>
+      <c r="A6" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="B6" s="14">
+        <v>700</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="14">
+        <v>28</v>
+      </c>
+      <c r="E6" s="14">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="19"/>
       <c r="I6" s="3"/>
       <c r="J6" s="2"/>
       <c r="K6" s="4"/>
@@ -2935,14 +2998,28 @@
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="22"/>
+      <c r="A7" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B7" s="14">
+        <v>695</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="14">
+        <v>28</v>
+      </c>
+      <c r="E7" s="14">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="19"/>
       <c r="I7" s="3"/>
       <c r="J7" s="2"/>
       <c r="K7" s="4"/>
@@ -2950,15 +3027,29 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="24"/>
+    <row r="8" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="B8" s="14">
+        <v>705</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="14">
+        <v>28</v>
+      </c>
+      <c r="E8" s="14">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="19"/>
       <c r="I8" s="3"/>
       <c r="J8" s="2"/>
       <c r="K8" s="4"/>
@@ -2967,14 +3058,28 @@
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="20"/>
+      <c r="A9" s="13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B9" s="14">
+        <v>705</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="14">
+        <v>38</v>
+      </c>
+      <c r="E9" s="14">
+        <v>75</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="19"/>
       <c r="I9" s="3"/>
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
@@ -2983,14 +3088,28 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="22"/>
+      <c r="A10" s="18">
+        <v>3</v>
+      </c>
+      <c r="B10" s="14">
+        <v>715</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="14">
+        <v>38</v>
+      </c>
+      <c r="E10" s="14">
+        <v>82</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="19"/>
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
@@ -2999,14 +3118,28 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="22"/>
+      <c r="A11" s="13">
+        <v>4</v>
+      </c>
+      <c r="B11" s="14">
+        <v>720</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="14">
+        <v>42</v>
+      </c>
+      <c r="E11" s="14">
+        <v>133</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="19"/>
       <c r="I11" s="3"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
@@ -3015,14 +3148,28 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="22"/>
+      <c r="A12" s="13">
+        <v>5.5</v>
+      </c>
+      <c r="B12" s="14">
+        <v>720</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="14">
+        <v>42</v>
+      </c>
+      <c r="E12" s="14">
+        <v>133</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="19"/>
       <c r="I12" s="3"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
@@ -3031,14 +3178,28 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="22"/>
+      <c r="A13" s="13">
+        <v>7.5</v>
+      </c>
+      <c r="B13" s="14">
+        <v>720</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="14">
+        <v>42</v>
+      </c>
+      <c r="E13" s="14">
+        <v>158</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="19"/>
       <c r="I13" s="3"/>
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
@@ -3046,123 +3207,193 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="24"/>
+    <row r="14" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14">
+        <v>720</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="14">
+        <v>48</v>
+      </c>
+      <c r="E14" s="14">
+        <v>210</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="19"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="20"/>
+      <c r="A15" s="18">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>730</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2">
+        <v>55</v>
+      </c>
+      <c r="E15" s="2">
+        <v>282</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="19"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="22"/>
+      <c r="A16" s="18">
+        <v>18.5</v>
+      </c>
+      <c r="B16" s="2">
+        <v>735</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2">
+        <v>60</v>
+      </c>
+      <c r="E16" s="2">
+        <v>360</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="19"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="22"/>
+      <c r="A17" s="18">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2">
+        <v>740</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2">
+        <v>60</v>
+      </c>
+      <c r="E17" s="2">
+        <v>375</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="19"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="22"/>
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20">
+        <v>30</v>
+      </c>
+      <c r="B18" s="9">
+        <v>735</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="9">
+        <v>70</v>
+      </c>
+      <c r="E18" s="9">
+        <v>510</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="21"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="22"/>
+      <c r="H19" s="32"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="22"/>
+      <c r="H20" s="32"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="32"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="22"/>
+      <c r="H22" s="32"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
+    <row r="23" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
@@ -3206,6 +3437,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:H1"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>